<commit_message>
git push origin main
</commit_message>
<xml_diff>
--- a/pknow/public/template.xlsx
+++ b/pknow/public/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\intan\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sahar\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C44775C-244D-477D-8D3C-BBCD4895F18F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8E846770-CB23-4AA9-88B5-7A52D941B79C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7BCF6A21-73E3-4667-B9AC-727DCDF25687}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="14595" xr2:uid="{7BCF6A21-73E3-4667-B9AC-727DCDF25687}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,23 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>No</t>
   </si>
@@ -48,9 +59,6 @@
     <t>Essay</t>
   </si>
   <si>
-    <t>5,0,0,0</t>
-  </si>
-  <si>
     <t>Pilgan</t>
   </si>
   <si>
@@ -67,6 +75,27 @@
   </si>
   <si>
     <t>Buatkan program java dengan tema apotek!</t>
+  </si>
+  <si>
+    <t>Digunakan untuk Soal Pilihan Ganda Tipe Tunggal</t>
+  </si>
+  <si>
+    <t>Digunakan untuk Soal Pilihan Ganda Tipe Jamak</t>
+  </si>
+  <si>
+    <t>Digunakan untuk Soal Praktikum</t>
+  </si>
+  <si>
+    <t>Digunakan untuk Soal Essai</t>
+  </si>
+  <si>
+    <t>Basis Data,PRG  5,PRG 6, Psikologi</t>
+  </si>
+  <si>
+    <t>25,0,0,10</t>
+  </si>
+  <si>
+    <t>25,0,0,0</t>
   </si>
 </sst>
 </file>
@@ -131,6 +160,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -450,29 +483,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB62D5FB-B7E1-41E2-A16F-8EE0975BDB54}">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="64.44140625" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="64.46484375" customWidth="1"/>
+    <col min="3" max="3" width="15.46484375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="131.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5546875" customWidth="1"/>
-    <col min="6" max="6" width="35.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5" customWidth="1"/>
+    <col min="5" max="5" width="12.53125" customWidth="1"/>
+    <col min="6" max="6" width="35.46484375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.19921875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="122.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="58.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="122.86328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="58.86328125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -487,7 +520,7 @@
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -501,13 +534,13 @@
         <v>2</v>
       </c>
       <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>1</v>
       </c>
@@ -515,16 +548,19 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>7</v>
+        <v>19</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>2</v>
       </c>
@@ -537,19 +573,42 @@
       <c r="F4">
         <v>15</v>
       </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F5">
-        <v>10</v>
+        <v>25</v>
+      </c>
+      <c r="G5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>